<commit_message>
Logboek, Userstories sprint 3
For progress on the site go to

https://github.com/EdgeworthWright/MyBand
</commit_message>
<xml_diff>
--- a/doc/userstories.xlsx
+++ b/doc/userstories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED60437E-87C3-46FF-8C72-870A6040BB13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA72A9C-F4B2-44EA-A1D6-1EABC95FFD33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="38">
   <si>
     <t>Done</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Content kunnen verwijderen</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -187,10 +190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -644,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,9 +684,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
+      <c r="F2" s="3"/>
       <c r="H2" t="s">
         <v>11</v>
       </c>
@@ -727,7 +729,7 @@
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
@@ -773,7 +775,7 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -793,7 +795,7 @@
         <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -847,7 +849,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>31</v>
@@ -873,7 +875,7 @@
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -890,7 +892,7 @@
         <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -907,7 +909,7 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -924,7 +926,7 @@
         <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>